<commit_message>
First working version that re-organizes files of a dataset into their class folders
</commit_message>
<xml_diff>
--- a/pytorch/data/cat_dog_small/cat_dog_small_annotations.xlsx
+++ b/pytorch/data/cat_dog_small/cat_dog_small_annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mxagar/nexo/git_repositories/templates/pytorch/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msagardia\play\git_repositories\templates\pytorch\data\cat_dog_small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F501F0B8-FDBB-624C-842E-20568217B1DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D6C1D2-748F-435D-9107-85DF3EF69932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="2000" windowWidth="28040" windowHeight="17440" xr2:uid="{9ED6C3E9-B00F-374C-A972-9C73B11BE202}"/>
+    <workbookView xWindow="7890" yWindow="2640" windowWidth="21600" windowHeight="11505" xr2:uid="{9ED6C3E9-B00F-374C-A972-9C73B11BE202}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -186,13 +185,13 @@
     <t>dog.250.jpg</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
     <t>Cat</t>
   </si>
   <si>
     <t>Dog</t>
+  </si>
+  <si>
+    <t>Filename</t>
   </si>
 </sst>
 </file>
@@ -546,24 +545,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CE4BBF-664A-654F-8303-FF46351643AB}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C27:C51"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -574,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -585,7 +582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -596,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -607,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -618,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -629,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -640,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -651,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -662,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -673,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -684,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -695,7 +692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -706,7 +703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -717,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -728,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -739,7 +736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -750,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -761,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -772,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -783,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -794,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -805,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -816,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -827,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -838,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -849,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -860,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -871,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -882,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -893,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -904,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -915,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -926,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -937,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -948,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -959,7 +956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -970,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -981,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -992,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1014,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1058,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1069,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1080,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>

</xml_diff>